<commit_message>
updated project 2 file
</commit_message>
<xml_diff>
--- a/Project 2.xlsx
+++ b/Project 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bugs\Desktop\CS 2400 Project 2\Project 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F64E4E9-EFBA-429C-BA78-219479757C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591D01AE-A9DF-4099-A773-1D320644961D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3795" yWindow="1485" windowWidth="13020" windowHeight="12210" xr2:uid="{ABF7A3E8-3E3B-4A3A-83C0-97D392ED3E9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABF7A3E8-3E3B-4A3A-83C0-97D392ED3E9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -621,7 +621,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>